<commit_message>
Tercer ejemplo con testng
</commit_message>
<xml_diff>
--- a/Usuarios.xlsx
+++ b/Usuarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\eclipse-workspace\ExampleLogin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE03C7BB-BE7B-4B61-A263-C027F8E01B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE582D0-7524-481A-9EA9-3A7CE5A1FC05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14715" yWindow="315" windowWidth="12990" windowHeight="8490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>Usuario</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>secret_sauce</t>
-  </si>
-  <si>
-    <t>s1ecret_sauce</t>
   </si>
   <si>
     <t>locked_out_user</t>
@@ -369,7 +366,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -387,7 +384,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -395,7 +392,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -403,7 +400,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -411,7 +408,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -419,10 +416,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>